<commit_message>
update account for medi
</commit_message>
<xml_diff>
--- a/meditations/docs/ToDos.xlsx
+++ b/meditations/docs/ToDos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -45,6 +45,9 @@
   <si>
     <t>实现从与服务器自动部署交易服务器设置</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>223账户的日盘log有输出  夜盘没有什么 是什么原因了？</t>
   </si>
 </sst>
 </file>
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -460,6 +463,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
+        <v>43108</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>